<commit_message>
update html interface update new bootstrap
</commit_message>
<xml_diff>
--- a/Sample/DataBase.xlsx
+++ b/Sample/DataBase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="18315" windowHeight="8280" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="18315" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="P01" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="278">
   <si>
     <t>收录卡包</t>
   </si>
@@ -696,9 +696,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>B01-034</t>
-  </si>
-  <si>
     <t>ソードスナイパー　リゲル</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -820,10 +817,6 @@
   </si>
   <si>
     <t>B03「五帝龙降临」</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>E02「日本一软件」</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1046,10 +1039,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>部分卡片同时具备多个种族。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>卡片描述与编号对应，卡片解说和官方裁定与卡名对应。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1428,6 +1417,46 @@
   <si>
     <t>同名卡仅显示第一个版本的搜索结果。排列顺序按编号。</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E02「日本一软件」</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>版本</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B01-034</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>（闪卡）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>部分卡片同时具备多个种族。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>版本</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>版本</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>（闪卡）</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>（吕布）</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>（世罗）</t>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2079,37 +2108,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="2.125" customWidth="1"/>
-    <col min="3" max="3" width="5.875" customWidth="1"/>
-    <col min="4" max="4" width="15.75" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="3.125" customWidth="1"/>
-    <col min="7" max="7" width="3.625" customWidth="1"/>
-    <col min="8" max="8" width="6.875" customWidth="1"/>
-    <col min="9" max="9" width="3.625" customWidth="1"/>
-    <col min="10" max="10" width="5.125" customWidth="1"/>
-    <col min="11" max="11" width="2.625" customWidth="1"/>
-    <col min="12" max="12" width="32.25" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="32.25" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="22" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.25" customWidth="1"/>
-    <col min="17" max="17" width="15.875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="2" customWidth="1"/>
-    <col min="19" max="19" width="27.75" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="5.875" customWidth="1"/>
+    <col min="5" max="5" width="15.75" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="3.125" customWidth="1"/>
+    <col min="8" max="8" width="3.625" customWidth="1"/>
+    <col min="9" max="9" width="6.875" customWidth="1"/>
+    <col min="10" max="10" width="3.625" customWidth="1"/>
+    <col min="11" max="11" width="5.125" customWidth="1"/>
+    <col min="12" max="12" width="2.625" customWidth="1"/>
+    <col min="13" max="13" width="32.25" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="32.25" style="2" customWidth="1"/>
+    <col min="15" max="15" width="21.625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="22" style="2" customWidth="1"/>
+    <col min="17" max="17" width="20.25" customWidth="1"/>
+    <col min="18" max="18" width="15.875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="2" customWidth="1"/>
+    <col min="20" max="20" width="27.75" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2120,64 +2149,67 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="2" customFormat="1" ht="101.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" s="2" customFormat="1" ht="101.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
@@ -2185,22 +2217,20 @@
         <v>54</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>37</v>
@@ -2211,29 +2241,32 @@
       <c r="K2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="4" t="s">
         <v>37</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="T2" s="24" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="101.25" x14ac:dyDescent="0.15">
+      <c r="U2" s="24" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="101.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
@@ -2243,20 +2276,18 @@
       <c r="C3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>37</v>
@@ -2267,29 +2298,32 @@
       <c r="K3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="4" t="s">
         <v>37</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="24" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="123.75" x14ac:dyDescent="0.15">
+      <c r="U3" s="24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="123.75" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
@@ -2299,20 +2333,18 @@
       <c r="C4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>37</v>
@@ -2323,29 +2355,32 @@
       <c r="K4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="4" t="s">
         <v>37</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="Q4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="T4" s="24" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="101.25" x14ac:dyDescent="0.15">
+      <c r="U4" s="24" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="101.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>84</v>
       </c>
@@ -2355,20 +2390,18 @@
       <c r="C5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>37</v>
@@ -2379,26 +2412,29 @@
       <c r="K5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="123.75" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" ht="123.75" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>84</v>
       </c>
@@ -2408,20 +2444,18 @@
       <c r="C6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>37</v>
@@ -2432,22 +2466,25 @@
       <c r="K6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="4" t="s">
         <v>37</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="P6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="Q6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2460,37 +2497,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T2" sqref="T2:T4"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="2.125" customWidth="1"/>
-    <col min="3" max="3" width="5.875" customWidth="1"/>
-    <col min="4" max="4" width="15.75" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="3.125" customWidth="1"/>
-    <col min="7" max="7" width="3.625" customWidth="1"/>
-    <col min="8" max="8" width="6.875" customWidth="1"/>
-    <col min="9" max="9" width="3.625" customWidth="1"/>
-    <col min="10" max="10" width="5.125" customWidth="1"/>
-    <col min="11" max="11" width="2.625" customWidth="1"/>
-    <col min="12" max="12" width="32.25" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="32.25" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="22" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.25" customWidth="1"/>
-    <col min="17" max="17" width="15.875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="2" customWidth="1"/>
-    <col min="19" max="19" width="27.75" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="5.875" customWidth="1"/>
+    <col min="5" max="5" width="15.75" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="3.125" customWidth="1"/>
+    <col min="8" max="8" width="3.625" customWidth="1"/>
+    <col min="9" max="9" width="6.875" customWidth="1"/>
+    <col min="10" max="10" width="3.625" customWidth="1"/>
+    <col min="11" max="11" width="5.125" customWidth="1"/>
+    <col min="12" max="12" width="2.625" customWidth="1"/>
+    <col min="13" max="13" width="32.25" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="32.25" style="2" customWidth="1"/>
+    <col min="15" max="15" width="21.625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="22" style="2" customWidth="1"/>
+    <col min="17" max="17" width="20.25" customWidth="1"/>
+    <col min="18" max="18" width="15.875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="2" customWidth="1"/>
+    <col min="20" max="20" width="27.75" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2501,64 +2538,67 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="101.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" ht="101.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>
@@ -2568,20 +2608,18 @@
       <c r="C2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>67</v>
@@ -2592,29 +2630,32 @@
       <c r="K2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>19</v>
+      <c r="L2" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="T2" s="24" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="101.25" x14ac:dyDescent="0.15">
+      <c r="U2" s="24" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="101.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -2624,20 +2665,18 @@
       <c r="C3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>67</v>
@@ -2648,29 +2687,32 @@
       <c r="K3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>19</v>
+      <c r="L3" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="P3" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="24" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="112.5" x14ac:dyDescent="0.15">
+      <c r="U3" s="24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="112.5" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
@@ -2680,20 +2722,18 @@
       <c r="C4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>67</v>
@@ -2704,29 +2744,32 @@
       <c r="K4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>19</v>
+      <c r="L4" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="P4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="Q4" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="T4" s="24" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="112.5" x14ac:dyDescent="0.15">
+      <c r="U4" s="24" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="112.5" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>86</v>
       </c>
@@ -2736,20 +2779,18 @@
       <c r="C5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>67</v>
@@ -2760,26 +2801,29 @@
       <c r="K5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>19</v>
+      <c r="L5" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="P5" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="112.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" ht="112.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>86</v>
       </c>
@@ -2789,20 +2833,18 @@
       <c r="C6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>67</v>
@@ -2813,22 +2855,25 @@
       <c r="K6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>19</v>
+      <c r="L6" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="P6" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="Q6" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2841,37 +2886,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R10" sqref="R10"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="2.125" customWidth="1"/>
-    <col min="3" max="3" width="5.875" customWidth="1"/>
-    <col min="4" max="4" width="15.75" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="3.125" customWidth="1"/>
-    <col min="7" max="7" width="3.625" customWidth="1"/>
-    <col min="8" max="8" width="6.875" customWidth="1"/>
-    <col min="9" max="9" width="3.625" customWidth="1"/>
-    <col min="10" max="10" width="5.125" customWidth="1"/>
-    <col min="11" max="11" width="2.625" customWidth="1"/>
-    <col min="12" max="12" width="32.25" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="32.25" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="22" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.25" customWidth="1"/>
-    <col min="17" max="17" width="15.875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="2" customWidth="1"/>
-    <col min="19" max="19" width="27.75" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="5.875" customWidth="1"/>
+    <col min="5" max="5" width="15.75" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="3.125" customWidth="1"/>
+    <col min="8" max="8" width="3.625" customWidth="1"/>
+    <col min="9" max="9" width="6.875" customWidth="1"/>
+    <col min="10" max="10" width="3.625" customWidth="1"/>
+    <col min="11" max="11" width="5.125" customWidth="1"/>
+    <col min="12" max="12" width="2.625" customWidth="1"/>
+    <col min="13" max="13" width="32.25" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="32.25" style="2" customWidth="1"/>
+    <col min="15" max="15" width="21.625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="22" style="2" customWidth="1"/>
+    <col min="17" max="17" width="20.25" customWidth="1"/>
+    <col min="18" max="18" width="15.875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="2" customWidth="1"/>
+    <col min="20" max="20" width="27.75" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2882,64 +2927,67 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>138</v>
       </c>
@@ -2947,58 +2995,123 @@
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="4">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4">
+        <v>6000</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="I2" s="4">
+      <c r="N2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="4">
         <v>5</v>
       </c>
-      <c r="J2" s="4">
+      <c r="K3" s="4">
         <v>6000</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M3" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O3" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="P3" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q3" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="S3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>166</v>
+      <c r="V3" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3010,37 +3123,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IU3"/>
+  <dimension ref="A1:IV4"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="2.125" customWidth="1"/>
-    <col min="3" max="3" width="5.875" customWidth="1"/>
-    <col min="4" max="4" width="15.75" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="3.125" customWidth="1"/>
-    <col min="7" max="7" width="3.625" customWidth="1"/>
-    <col min="8" max="8" width="6.875" customWidth="1"/>
-    <col min="9" max="9" width="3.625" customWidth="1"/>
-    <col min="10" max="10" width="5.125" customWidth="1"/>
-    <col min="11" max="11" width="2.625" customWidth="1"/>
-    <col min="12" max="12" width="32.25" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="32.25" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="22" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.25" customWidth="1"/>
-    <col min="17" max="17" width="15.875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="2" customWidth="1"/>
-    <col min="19" max="19" width="27.75" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="5.875" customWidth="1"/>
+    <col min="5" max="5" width="15.75" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="3.125" customWidth="1"/>
+    <col min="8" max="8" width="3.625" customWidth="1"/>
+    <col min="9" max="9" width="6.875" customWidth="1"/>
+    <col min="10" max="10" width="3.625" customWidth="1"/>
+    <col min="11" max="11" width="5.125" customWidth="1"/>
+    <col min="12" max="12" width="2.625" customWidth="1"/>
+    <col min="13" max="13" width="32.25" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="32.25" style="2" customWidth="1"/>
+    <col min="15" max="15" width="21.625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="22" style="2" customWidth="1"/>
+    <col min="17" max="17" width="20.25" customWidth="1"/>
+    <col min="18" max="18" width="15.875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="2" customWidth="1"/>
+    <col min="20" max="20" width="27.75" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:256" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3051,182 +3164,186 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:255" s="24" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:256" s="24" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A2" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>243</v>
+      </c>
+      <c r="I2" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="J2" s="32">
+        <v>3</v>
+      </c>
+      <c r="K2" s="31">
+        <v>5000</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="M2" s="24" t="s">
         <v>259</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="N2" s="24" t="s">
         <v>260</v>
       </c>
-      <c r="F2" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>246</v>
-      </c>
-      <c r="H2" s="31" t="s">
+      <c r="O2" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="I2" s="32">
-        <v>3</v>
-      </c>
-      <c r="J2" s="31">
-        <v>5000</v>
-      </c>
-      <c r="K2" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="L2" s="24" t="s">
+      <c r="P2" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="Q2" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="S2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="29"/>
+      <c r="V2" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="O2" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>266</v>
-      </c>
-      <c r="R2" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="S2" s="29"/>
-      <c r="U2" s="24" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="3" spans="1:255" ht="146.25" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:256" ht="146.25" x14ac:dyDescent="0.15">
       <c r="A3" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="H3" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="I3" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="J3" s="32">
+        <v>6</v>
+      </c>
+      <c r="K3" s="31">
+        <v>7500</v>
+      </c>
+      <c r="L3" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="M3" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="N3" s="26" t="s">
         <v>232</v>
       </c>
-      <c r="I3" s="32">
-        <v>6</v>
-      </c>
-      <c r="J3" s="31">
-        <v>7500</v>
-      </c>
-      <c r="K3" s="31" t="s">
+      <c r="O3" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="P3" s="26" t="s">
         <v>234</v>
       </c>
-      <c r="M3" s="26" t="s">
+      <c r="Q3" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="N3" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="O3" s="26" t="s">
+      <c r="T3" s="29"/>
+      <c r="U3" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="P3" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24" t="s">
+      <c r="V3" s="24"/>
+      <c r="W3" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="S3" s="29"/>
-      <c r="T3" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="W3" s="24"/>
       <c r="X3" s="24"/>
       <c r="Y3" s="24"/>
       <c r="Z3" s="24"/>
@@ -3459,6 +3576,305 @@
       <c r="IS3" s="24"/>
       <c r="IT3" s="24"/>
       <c r="IU3" s="24"/>
+      <c r="IV3" s="24"/>
+    </row>
+    <row r="4" spans="1:256" ht="146.25" x14ac:dyDescent="0.15">
+      <c r="A4" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="J4" s="32">
+        <v>6</v>
+      </c>
+      <c r="K4" s="31">
+        <v>7500</v>
+      </c>
+      <c r="L4" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="O4" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="P4" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q4" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="T4" s="29"/>
+      <c r="U4" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="24"/>
+      <c r="AH4" s="24"/>
+      <c r="AI4" s="24"/>
+      <c r="AJ4" s="24"/>
+      <c r="AK4" s="24"/>
+      <c r="AL4" s="24"/>
+      <c r="AM4" s="24"/>
+      <c r="AN4" s="24"/>
+      <c r="AO4" s="24"/>
+      <c r="AP4" s="24"/>
+      <c r="AQ4" s="24"/>
+      <c r="AR4" s="24"/>
+      <c r="AS4" s="24"/>
+      <c r="AT4" s="24"/>
+      <c r="AU4" s="24"/>
+      <c r="AV4" s="24"/>
+      <c r="AW4" s="24"/>
+      <c r="AX4" s="24"/>
+      <c r="AY4" s="24"/>
+      <c r="AZ4" s="24"/>
+      <c r="BA4" s="24"/>
+      <c r="BB4" s="24"/>
+      <c r="BC4" s="24"/>
+      <c r="BD4" s="24"/>
+      <c r="BE4" s="24"/>
+      <c r="BF4" s="24"/>
+      <c r="BG4" s="24"/>
+      <c r="BH4" s="24"/>
+      <c r="BI4" s="24"/>
+      <c r="BJ4" s="24"/>
+      <c r="BK4" s="24"/>
+      <c r="BL4" s="24"/>
+      <c r="BM4" s="24"/>
+      <c r="BN4" s="24"/>
+      <c r="BO4" s="24"/>
+      <c r="BP4" s="24"/>
+      <c r="BQ4" s="24"/>
+      <c r="BR4" s="24"/>
+      <c r="BS4" s="24"/>
+      <c r="BT4" s="24"/>
+      <c r="BU4" s="24"/>
+      <c r="BV4" s="24"/>
+      <c r="BW4" s="24"/>
+      <c r="BX4" s="24"/>
+      <c r="BY4" s="24"/>
+      <c r="BZ4" s="24"/>
+      <c r="CA4" s="24"/>
+      <c r="CB4" s="24"/>
+      <c r="CC4" s="24"/>
+      <c r="CD4" s="24"/>
+      <c r="CE4" s="24"/>
+      <c r="CF4" s="24"/>
+      <c r="CG4" s="24"/>
+      <c r="CH4" s="24"/>
+      <c r="CI4" s="24"/>
+      <c r="CJ4" s="24"/>
+      <c r="CK4" s="24"/>
+      <c r="CL4" s="24"/>
+      <c r="CM4" s="24"/>
+      <c r="CN4" s="24"/>
+      <c r="CO4" s="24"/>
+      <c r="CP4" s="24"/>
+      <c r="CQ4" s="24"/>
+      <c r="CR4" s="24"/>
+      <c r="CS4" s="24"/>
+      <c r="CT4" s="24"/>
+      <c r="CU4" s="24"/>
+      <c r="CV4" s="24"/>
+      <c r="CW4" s="24"/>
+      <c r="CX4" s="24"/>
+      <c r="CY4" s="24"/>
+      <c r="CZ4" s="24"/>
+      <c r="DA4" s="24"/>
+      <c r="DB4" s="24"/>
+      <c r="DC4" s="24"/>
+      <c r="DD4" s="24"/>
+      <c r="DE4" s="24"/>
+      <c r="DF4" s="24"/>
+      <c r="DG4" s="24"/>
+      <c r="DH4" s="24"/>
+      <c r="DI4" s="24"/>
+      <c r="DJ4" s="24"/>
+      <c r="DK4" s="24"/>
+      <c r="DL4" s="24"/>
+      <c r="DM4" s="24"/>
+      <c r="DN4" s="24"/>
+      <c r="DO4" s="24"/>
+      <c r="DP4" s="24"/>
+      <c r="DQ4" s="24"/>
+      <c r="DR4" s="24"/>
+      <c r="DS4" s="24"/>
+      <c r="DT4" s="24"/>
+      <c r="DU4" s="24"/>
+      <c r="DV4" s="24"/>
+      <c r="DW4" s="24"/>
+      <c r="DX4" s="24"/>
+      <c r="DY4" s="24"/>
+      <c r="DZ4" s="24"/>
+      <c r="EA4" s="24"/>
+      <c r="EB4" s="24"/>
+      <c r="EC4" s="24"/>
+      <c r="ED4" s="24"/>
+      <c r="EE4" s="24"/>
+      <c r="EF4" s="24"/>
+      <c r="EG4" s="24"/>
+      <c r="EH4" s="24"/>
+      <c r="EI4" s="24"/>
+      <c r="EJ4" s="24"/>
+      <c r="EK4" s="24"/>
+      <c r="EL4" s="24"/>
+      <c r="EM4" s="24"/>
+      <c r="EN4" s="24"/>
+      <c r="EO4" s="24"/>
+      <c r="EP4" s="24"/>
+      <c r="EQ4" s="24"/>
+      <c r="ER4" s="24"/>
+      <c r="ES4" s="24"/>
+      <c r="ET4" s="24"/>
+      <c r="EU4" s="24"/>
+      <c r="EV4" s="24"/>
+      <c r="EW4" s="24"/>
+      <c r="EX4" s="24"/>
+      <c r="EY4" s="24"/>
+      <c r="EZ4" s="24"/>
+      <c r="FA4" s="24"/>
+      <c r="FB4" s="24"/>
+      <c r="FC4" s="24"/>
+      <c r="FD4" s="24"/>
+      <c r="FE4" s="24"/>
+      <c r="FF4" s="24"/>
+      <c r="FG4" s="24"/>
+      <c r="FH4" s="24"/>
+      <c r="FI4" s="24"/>
+      <c r="FJ4" s="24"/>
+      <c r="FK4" s="24"/>
+      <c r="FL4" s="24"/>
+      <c r="FM4" s="24"/>
+      <c r="FN4" s="24"/>
+      <c r="FO4" s="24"/>
+      <c r="FP4" s="24"/>
+      <c r="FQ4" s="24"/>
+      <c r="FR4" s="24"/>
+      <c r="FS4" s="24"/>
+      <c r="FT4" s="24"/>
+      <c r="FU4" s="24"/>
+      <c r="FV4" s="24"/>
+      <c r="FW4" s="24"/>
+      <c r="FX4" s="24"/>
+      <c r="FY4" s="24"/>
+      <c r="FZ4" s="24"/>
+      <c r="GA4" s="24"/>
+      <c r="GB4" s="24"/>
+      <c r="GC4" s="24"/>
+      <c r="GD4" s="24"/>
+      <c r="GE4" s="24"/>
+      <c r="GF4" s="24"/>
+      <c r="GG4" s="24"/>
+      <c r="GH4" s="24"/>
+      <c r="GI4" s="24"/>
+      <c r="GJ4" s="24"/>
+      <c r="GK4" s="24"/>
+      <c r="GL4" s="24"/>
+      <c r="GM4" s="24"/>
+      <c r="GN4" s="24"/>
+      <c r="GO4" s="24"/>
+      <c r="GP4" s="24"/>
+      <c r="GQ4" s="24"/>
+      <c r="GR4" s="24"/>
+      <c r="GS4" s="24"/>
+      <c r="GT4" s="24"/>
+      <c r="GU4" s="24"/>
+      <c r="GV4" s="24"/>
+      <c r="GW4" s="24"/>
+      <c r="GX4" s="24"/>
+      <c r="GY4" s="24"/>
+      <c r="GZ4" s="24"/>
+      <c r="HA4" s="24"/>
+      <c r="HB4" s="24"/>
+      <c r="HC4" s="24"/>
+      <c r="HD4" s="24"/>
+      <c r="HE4" s="24"/>
+      <c r="HF4" s="24"/>
+      <c r="HG4" s="24"/>
+      <c r="HH4" s="24"/>
+      <c r="HI4" s="24"/>
+      <c r="HJ4" s="24"/>
+      <c r="HK4" s="24"/>
+      <c r="HL4" s="24"/>
+      <c r="HM4" s="24"/>
+      <c r="HN4" s="24"/>
+      <c r="HO4" s="24"/>
+      <c r="HP4" s="24"/>
+      <c r="HQ4" s="24"/>
+      <c r="HR4" s="24"/>
+      <c r="HS4" s="24"/>
+      <c r="HT4" s="24"/>
+      <c r="HU4" s="24"/>
+      <c r="HV4" s="24"/>
+      <c r="HW4" s="24"/>
+      <c r="HX4" s="24"/>
+      <c r="HY4" s="24"/>
+      <c r="HZ4" s="24"/>
+      <c r="IA4" s="24"/>
+      <c r="IB4" s="24"/>
+      <c r="IC4" s="24"/>
+      <c r="ID4" s="24"/>
+      <c r="IE4" s="24"/>
+      <c r="IF4" s="24"/>
+      <c r="IG4" s="24"/>
+      <c r="IH4" s="24"/>
+      <c r="II4" s="24"/>
+      <c r="IJ4" s="24"/>
+      <c r="IK4" s="24"/>
+      <c r="IL4" s="24"/>
+      <c r="IM4" s="24"/>
+      <c r="IN4" s="24"/>
+      <c r="IO4" s="24"/>
+      <c r="IP4" s="24"/>
+      <c r="IQ4" s="24"/>
+      <c r="IR4" s="24"/>
+      <c r="IS4" s="24"/>
+      <c r="IT4" s="24"/>
+      <c r="IU4" s="24"/>
+      <c r="IV4" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
@@ -3469,37 +3885,37 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IU2"/>
+  <dimension ref="A1:IV2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="2.125" customWidth="1"/>
-    <col min="3" max="3" width="5.875" customWidth="1"/>
-    <col min="4" max="4" width="15.75" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="3.125" customWidth="1"/>
-    <col min="7" max="7" width="3.625" customWidth="1"/>
-    <col min="8" max="8" width="6.875" customWidth="1"/>
-    <col min="9" max="9" width="3.625" customWidth="1"/>
-    <col min="10" max="10" width="5.125" customWidth="1"/>
-    <col min="11" max="11" width="2.625" customWidth="1"/>
-    <col min="12" max="12" width="32.25" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="32.25" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="22" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.25" customWidth="1"/>
-    <col min="17" max="17" width="15.875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="2" customWidth="1"/>
-    <col min="19" max="19" width="27.75" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="5.875" customWidth="1"/>
+    <col min="5" max="5" width="15.75" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="3.125" customWidth="1"/>
+    <col min="8" max="8" width="3.625" customWidth="1"/>
+    <col min="9" max="9" width="6.875" customWidth="1"/>
+    <col min="10" max="10" width="3.625" customWidth="1"/>
+    <col min="11" max="11" width="5.125" customWidth="1"/>
+    <col min="12" max="12" width="2.625" customWidth="1"/>
+    <col min="13" max="13" width="32.25" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="32.25" style="2" customWidth="1"/>
+    <col min="15" max="15" width="21.625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="22" style="2" customWidth="1"/>
+    <col min="17" max="17" width="20.25" customWidth="1"/>
+    <col min="18" max="18" width="15.875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="2" customWidth="1"/>
+    <col min="20" max="20" width="27.75" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:256" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3510,122 +3926,125 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:255" ht="78.75" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:256" ht="78.75" x14ac:dyDescent="0.15">
       <c r="A2" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C2" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="H2" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="I2" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="J2" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="K2" s="27">
+        <v>3500</v>
+      </c>
+      <c r="L2" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="M2" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="N2" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="O2" s="26" t="s">
         <v>248</v>
       </c>
-      <c r="J2" s="27">
-        <v>3500</v>
-      </c>
-      <c r="K2" s="27" t="s">
+      <c r="P2" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="Q2" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="M2" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="N2" s="26" t="s">
+      <c r="R2" s="24"/>
+      <c r="S2" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="O2" s="24" t="s">
-        <v>252</v>
-      </c>
-      <c r="P2" s="26" t="s">
+      <c r="T2" s="29"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="26" t="s">
-        <v>254</v>
-      </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="V2" s="24"/>
       <c r="W2" s="24"/>
       <c r="X2" s="24"/>
       <c r="Y2" s="24"/>
@@ -3859,6 +4278,7 @@
       <c r="IS2" s="24"/>
       <c r="IT2" s="24"/>
       <c r="IU2" s="24"/>
+      <c r="IV2" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
@@ -3869,11 +4289,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IU3"/>
+  <dimension ref="A1:IV3"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -3881,25 +4301,25 @@
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="2.125" customWidth="1"/>
     <col min="3" max="3" width="5.875" customWidth="1"/>
-    <col min="4" max="4" width="15.75" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="3.125" customWidth="1"/>
-    <col min="7" max="7" width="3.625" customWidth="1"/>
-    <col min="8" max="8" width="6.875" customWidth="1"/>
-    <col min="9" max="9" width="3.625" customWidth="1"/>
-    <col min="10" max="10" width="5.125" customWidth="1"/>
-    <col min="11" max="11" width="2.625" customWidth="1"/>
-    <col min="12" max="12" width="32.25" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="32.25" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="22" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.25" customWidth="1"/>
-    <col min="17" max="17" width="15.875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="2" customWidth="1"/>
-    <col min="19" max="19" width="27.75" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="15.75" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="3.125" customWidth="1"/>
+    <col min="8" max="8" width="3.625" customWidth="1"/>
+    <col min="9" max="9" width="6.875" customWidth="1"/>
+    <col min="10" max="10" width="3.625" customWidth="1"/>
+    <col min="11" max="11" width="5.125" customWidth="1"/>
+    <col min="12" max="12" width="2.625" customWidth="1"/>
+    <col min="13" max="13" width="32.25" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="32.25" style="2" customWidth="1"/>
+    <col min="15" max="15" width="21.625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="22" style="2" customWidth="1"/>
+    <col min="17" max="17" width="20.25" customWidth="1"/>
+    <col min="18" max="18" width="15.875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="2" customWidth="1"/>
+    <col min="20" max="20" width="27.75" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:256" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3913,111 +4333,116 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:255" ht="78.75" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:256" ht="78.75" x14ac:dyDescent="0.15">
       <c r="A2" s="24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="E2" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="G2" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="H2" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="I2" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="J2" s="27">
+        <v>4</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="L2" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="M2" s="26"/>
+      <c r="N2" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="I2" s="27">
-        <v>4</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="K2" s="27" t="s">
+      <c r="O2" s="28"/>
+      <c r="P2" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="24" t="s">
+      <c r="Q2" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="N2" s="28"/>
-      <c r="O2" s="26" t="s">
+      <c r="R2" s="24"/>
+      <c r="S2" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="P2" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24" t="s">
-        <v>218</v>
-      </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="24"/>
+      <c r="T2" s="29"/>
       <c r="U2" s="24"/>
       <c r="V2" s="24"/>
       <c r="W2" s="24"/>
@@ -4253,58 +4678,61 @@
       <c r="IS2" s="24"/>
       <c r="IT2" s="24"/>
       <c r="IU2" s="24"/>
-    </row>
-    <row r="3" spans="1:255" ht="78.75" x14ac:dyDescent="0.15">
+      <c r="IV2" s="24"/>
+    </row>
+    <row r="3" spans="1:256" ht="78.75" x14ac:dyDescent="0.15">
       <c r="A3" s="24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="E3" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="F3" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="G3" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="H3" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="I3" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="J3" s="27">
+        <v>4</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="L3" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="M3" s="26"/>
+      <c r="N3" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="I3" s="27">
-        <v>4</v>
-      </c>
-      <c r="J3" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="K3" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="L3" s="26"/>
-      <c r="M3" s="24" t="s">
+      <c r="O3" s="28"/>
+      <c r="P3" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q3" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="N3" s="28"/>
-      <c r="O3" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="P3" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="S3" s="29"/>
-      <c r="T3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="T3" s="29"/>
       <c r="U3" s="24"/>
       <c r="V3" s="24"/>
       <c r="W3" s="24"/>
@@ -4540,6 +4968,7 @@
       <c r="IS3" s="24"/>
       <c r="IT3" s="24"/>
       <c r="IU3" s="24"/>
+      <c r="IV3" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
@@ -4552,90 +4981,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="2" spans="11:12" x14ac:dyDescent="0.15">
       <c r="K2" s="21" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="11:12" x14ac:dyDescent="0.15">
       <c r="K3" s="21" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="11:12" x14ac:dyDescent="0.15">
       <c r="K4" s="21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="11:12" x14ac:dyDescent="0.15">
       <c r="K5" s="21" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="11:12" x14ac:dyDescent="0.15">
       <c r="K7" s="22" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="11:12" x14ac:dyDescent="0.15">
       <c r="L8" s="21" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="11:12" x14ac:dyDescent="0.15">
       <c r="L9" s="21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="11:12" x14ac:dyDescent="0.15">
       <c r="K11" s="21" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="11:12" x14ac:dyDescent="0.15">
       <c r="K13" s="21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="11:12" x14ac:dyDescent="0.15">
       <c r="K15" s="21" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="11:12" x14ac:dyDescent="0.15">
       <c r="L16" s="21" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="K18" s="23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="K19" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="K20" s="23" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="K21" s="23" t="s">
-        <v>221</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="K22" s="23" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.15">
@@ -4673,7 +5102,7 @@
         <v>93</v>
       </c>
       <c r="L24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M24" t="s">
         <v>94</v>
@@ -4705,10 +5134,10 @@
         <v>108</v>
       </c>
       <c r="L25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="N25" t="s">
         <v>142</v>
@@ -4731,13 +5160,13 @@
         <v>109</v>
       </c>
       <c r="L26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M26" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="N26" s="21" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="P26" t="s">
         <v>103</v>
@@ -4754,10 +5183,10 @@
         <v>110</v>
       </c>
       <c r="L27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="N27" t="s">
         <v>143</v>
@@ -4777,10 +5206,10 @@
         <v>111</v>
       </c>
       <c r="L28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="M28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="N28" t="s">
         <v>144</v>
@@ -4800,10 +5229,10 @@
         <v>112</v>
       </c>
       <c r="L29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="N29" t="s">
         <v>145</v>
@@ -4823,10 +5252,10 @@
         <v>113</v>
       </c>
       <c r="L30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="N30" t="s">
         <v>140</v>
@@ -4843,10 +5272,10 @@
         <v>114</v>
       </c>
       <c r="L31" t="s">
-        <v>172</v>
+        <v>268</v>
       </c>
       <c r="M31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="N31" t="s">
         <v>146</v>
@@ -4863,10 +5292,10 @@
         <v>115</v>
       </c>
       <c r="L32" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="N32" t="s">
         <v>147</v>
@@ -4883,10 +5312,10 @@
         <v>128</v>
       </c>
       <c r="L33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M33" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="N33" t="s">
         <v>148</v>
@@ -4900,10 +5329,10 @@
         <v>116</v>
       </c>
       <c r="L34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="4:14" x14ac:dyDescent="0.15">
@@ -4914,10 +5343,10 @@
         <v>117</v>
       </c>
       <c r="L35" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M35" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="4:14" x14ac:dyDescent="0.15">
@@ -4931,7 +5360,7 @@
         <v>133</v>
       </c>
       <c r="M36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="4:14" x14ac:dyDescent="0.15">
@@ -4945,7 +5374,7 @@
         <v>134</v>
       </c>
       <c r="M37" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="4:14" x14ac:dyDescent="0.15">
@@ -4959,7 +5388,7 @@
         <v>135</v>
       </c>
       <c r="M38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="4:14" x14ac:dyDescent="0.15">
@@ -4973,7 +5402,7 @@
         <v>136</v>
       </c>
       <c r="M39" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="4:14" x14ac:dyDescent="0.15">
@@ -4987,7 +5416,7 @@
         <v>137</v>
       </c>
       <c r="M40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="4:14" x14ac:dyDescent="0.15">
@@ -4998,10 +5427,10 @@
         <v>122</v>
       </c>
       <c r="L41" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="M41" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="4:14" x14ac:dyDescent="0.15">
@@ -5012,10 +5441,10 @@
         <v>123</v>
       </c>
       <c r="L42" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="4:14" x14ac:dyDescent="0.15">
@@ -5026,10 +5455,10 @@
         <v>130</v>
       </c>
       <c r="L43" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="M43" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="4:14" x14ac:dyDescent="0.15">
@@ -5040,10 +5469,10 @@
         <v>124</v>
       </c>
       <c r="L44" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M44" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="4:14" x14ac:dyDescent="0.15">
@@ -5054,10 +5483,10 @@
         <v>125</v>
       </c>
       <c r="L45" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M45" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="4:14" x14ac:dyDescent="0.15">
@@ -5065,10 +5494,10 @@
         <v>126</v>
       </c>
       <c r="L46" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="M46" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="4:14" x14ac:dyDescent="0.15">
@@ -5076,10 +5505,10 @@
         <v>127</v>
       </c>
       <c r="L47" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="M47" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="4:14" x14ac:dyDescent="0.15">
@@ -5087,10 +5516,10 @@
         <v>131</v>
       </c>
       <c r="L48" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M48" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="10:13" x14ac:dyDescent="0.15">
@@ -5098,26 +5527,26 @@
         <v>132</v>
       </c>
       <c r="L49" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M49" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="10:13" x14ac:dyDescent="0.15">
       <c r="L50" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M50" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" spans="10:13" x14ac:dyDescent="0.15">
       <c r="L51" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M51" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="10:13" x14ac:dyDescent="0.15">
@@ -5125,7 +5554,7 @@
         <v>149</v>
       </c>
       <c r="M52" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>